<commit_message>
update again get test data
</commit_message>
<xml_diff>
--- a/csci318.xlsx
+++ b/csci318.xlsx
@@ -6,9 +6,7 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Chinese" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Swedish" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Japanese" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="English" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -16,15 +14,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
-  <si>
-    <t>The name bugleweed is a common name which can refer to several unrelated plants:.</t>
-  </si>
-  <si>
-    <t>Bird vocalization includes both bird calls and bird songs..</t>
-  </si>
-  <si>
-    <t>Fireproofing is rendering something (structures, materials, etc.) resistant to fire, or incombustible; or material for use in making anything fire-proof..</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
+  <si>
+    <t>The abampere (abA), also called the biot (Bi) after Jean-Baptiste Biot, is the basic electromagnetic unit of electric current in the emu-cgs system of units (electromagnetic cgs).</t>
+  </si>
+  <si>
+    <t>In biology and human medicine, gravidity and parity are the number of times a female is or has been pregnant (gravidity) and carried the pregnancies to a viable gestational age (parity).</t>
+  </si>
+  <si>
+    <t>"Praseolite" redirects here.</t>
+  </si>
+  <si>
+    <t>The mineral cristobalite is a high-temperature polymorph of silica, meaning that it has the same chemical formula as quartz, SiO2, but a distinct crystal structure.</t>
+  </si>
+  <si>
+    <t>Exoteric refers to knowledge that is outside, and independent from, a person's experience and can be ascertained by anyone (related to common sense).</t>
+  </si>
+  <si>
+    <t>A groomsman (North America), or usher (British Isles) is one of the male attendants to the groom in a wedding ceremony.</t>
+  </si>
+  <si>
+    <t>In dynamical systems, intermittency is the irregular alternation of phases of apparently periodic and chaotic dynamics (Pomeau–Manneville dynamics), or different forms of chaotic dynamics (crisis-induced intermittency).</t>
   </si>
 </sst>
 </file>
@@ -360,7 +370,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -383,72 +393,24 @@
         <v>2</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>2</v>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>